<commit_message>
Practiced and noted CREATE USE SHOW DROP DESC keywords with tables and databases
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5C6EDC-65F7-41B2-B845-54426F5F43C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CE8A85-AEF4-4BEC-8B6F-BB3768CD429B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -420,26 +420,43 @@
     <t>To create table</t>
   </si>
   <si>
-    <t>CREATE TABLE mytable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop </t>
-  </si>
-  <si>
     <t>SHOW</t>
   </si>
   <si>
     <t>SHOW DATABASES</t>
   </si>
   <si>
+    <t>To get existing databases names</t>
+  </si>
+  <si>
+    <t>To get existing tables names</t>
+  </si>
+  <si>
+    <t>To delete database</t>
+  </si>
+  <si>
+    <t>To delete table</t>
+  </si>
+  <si>
+    <t>DROP DATABASE mydabase</t>
+  </si>
+  <si>
+    <t>DROP TABLE mytable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USE mydatabase;
+CREATE TABLE mytable
+(
+ name VARCHAR(100),
+    age INT
+);
+</t>
+  </si>
+  <si>
     <t>USE mydabases;
-SHOW TABLES</t>
-  </si>
-  <si>
-    <t>To get existing databases names</t>
-  </si>
-  <si>
-    <t>To get existing tables names</t>
+SHOW TABLES
+SHOW COLUMNS FROM mytable
+DESC mytable # DESC here means describe</t>
   </si>
 </sst>
 </file>
@@ -837,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,24 +892,24 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,14 +924,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>72</v>
+      <c r="D6" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,15 +940,21 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">

</xml_diff>

<commit_message>
Usage of NOT NULL, DEFAULT, AUTO_INCREMENT, PRIMARY KEY keywords while creating table
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CE8A85-AEF4-4BEC-8B6F-BB3768CD429B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8150350-B855-4650-9949-BB0A9EB826A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -444,19 +444,61 @@
     <t>DROP TABLE mytable</t>
   </si>
   <si>
-    <t xml:space="preserve">USE mydatabase;
-CREATE TABLE mytable
-(
- name VARCHAR(100),
-    age INT
-);
-</t>
-  </si>
-  <si>
     <t>USE mydabases;
 SHOW TABLES
 SHOW COLUMNS FROM mytable
 DESC mytable # DESC here means describe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT </t>
+  </si>
+  <si>
+    <t>To insert data into tables</t>
+  </si>
+  <si>
+    <t>INSERT INTO pastries(name, quantity) VALUES ('Chocolatecake', 6)</t>
+  </si>
+  <si>
+    <t>INSERT INTO pastries(name, quantity) VALUES ('venelacake', 6), ('strawberrycake', 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USE mydatabase;
+CREATE TABLE mytable
+(
+ name VARCHAR(100) NOT NULL,
+    age INT
+);
+</t>
+  </si>
+  <si>
+    <t>7. By default NULL will be given to columns. So that when we don’t specify the values NULL will be assigned as value</t>
+  </si>
+  <si>
+    <t>6. When creating a tables we should mention mandatory column names to be inserted while adding data to table by using NOT NULL keywords. So that when we don't specify values it gives 0 for INT and blank for VARCHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Using DEFAULT keyword. When we want to give a default name when there blank values is inserted. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">USE mydatabase;
+CREATE TABLE mytable
+(
+ name VARCHAR(100) DEFAULT 'unnamed',
+    age INT DEFAULT 99
+);
+</t>
+  </si>
+  <si>
+    <t>9. Use of PRIMARY KEY keyword. When we want a unique ID created for each data inserted we can use this PRIMARY KEY keyword</t>
+  </si>
+  <si>
+    <t>CREATE TABLE unique_cats(catID INT NOT NULL, name VARCHAR(20) DEFAULT 'unnamed', age INT, PRIMARY KEY (catID));</t>
+  </si>
+  <si>
+    <t>10. Use AUTO_INCREMENT keyword.</t>
+  </si>
+  <si>
+    <t>CREATE TABLE unique_cats(catID INT NOT NULL AUTO_INCREMENT, name VARCHAR(20) DEFAULT 'unnamed', age INT, PRIMARY KEY (catID));</t>
   </si>
 </sst>
 </file>
@@ -534,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -566,11 +608,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,10 +897,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +927,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="3"/>
@@ -891,7 +937,7 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>72</v>
       </c>
       <c r="B3" s="6"/>
@@ -903,13 +949,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,17 +971,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>68</v>
       </c>
       <c r="B7" s="6"/>
@@ -1203,6 +1249,22 @@
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1212,9 +1274,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A372CFD-6369-4C1F-9C7A-9162FAE256E2}">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="A2:B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1223,31 +1287,73 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Practice on CRUD queries
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8150350-B855-4650-9949-BB0A9EB826A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039DDABE-496B-4D44-BA48-59D1ECFD0B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -474,12 +474,6 @@
     <t>7. By default NULL will be given to columns. So that when we don’t specify the values NULL will be assigned as value</t>
   </si>
   <si>
-    <t>6. When creating a tables we should mention mandatory column names to be inserted while adding data to table by using NOT NULL keywords. So that when we don't specify values it gives 0 for INT and blank for VARCHAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Using DEFAULT keyword. When we want to give a default name when there blank values is inserted. </t>
-  </si>
-  <si>
     <t xml:space="preserve">USE mydatabase;
 CREATE TABLE mytable
 (
@@ -489,23 +483,186 @@
 </t>
   </si>
   <si>
-    <t>9. Use of PRIMARY KEY keyword. When we want a unique ID created for each data inserted we can use this PRIMARY KEY keyword</t>
-  </si>
-  <si>
     <t>CREATE TABLE unique_cats(catID INT NOT NULL, name VARCHAR(20) DEFAULT 'unnamed', age INT, PRIMARY KEY (catID));</t>
   </si>
   <si>
-    <t>10. Use AUTO_INCREMENT keyword.</t>
-  </si>
-  <si>
     <t>CREATE TABLE unique_cats(catID INT NOT NULL AUTO_INCREMENT, name VARCHAR(20) DEFAULT 'unnamed', age INT, PRIMARY KEY (catID));</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>UPDATE cats SET breed='Shorthair' WHERE breed='tabby'</t>
+  </si>
+  <si>
+    <t>UPDATE cats SET age=12 WHERE breed='Maine Coon'</t>
+  </si>
+  <si>
+    <t>To update data in existing tables</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <r>
+      <t>DELETE FROM cats WHERE name=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Egg'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>To delete rows</t>
+  </si>
+  <si>
+    <t>To delete all rows in a table</t>
+  </si>
+  <si>
+    <t>DELETE FROM cats</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10. Use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AUTO_INCREMENT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyword.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9. Use of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PRIMARY KEY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyword. When we want a unique ID created for each data inserted we can use this PRIMARY KEY keyword</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8. Using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyword. When we want to give a default name when there blank values is inserted. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6. When creating a tables we should mention mandatory column names to be inserted while adding data to table by using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keywords. So that when we don't specify values it gives 0 for INT and blank for VARCHAR</t>
+    </r>
+  </si>
+  <si>
+    <t>UPDATE shirts SET color='off white', shirt_size='X' WHERE color='white'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTO </t>
+  </si>
+  <si>
+    <t>VALUES</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>update MULTIPLE colomuns with ,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +677,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1C1D1F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF2D907F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -536,7 +705,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -572,11 +741,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -617,6 +795,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,11 +1081,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,20 +1434,86 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1274,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A372CFD-6369-4C1F-9C7A-9162FAE256E2}">
-  <dimension ref="A2:B11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="A2:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,31 +1536,64 @@
     <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18"/>
+      <c r="C2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18"/>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
+      <c r="C4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
+      <c r="C5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>65</v>
       </c>
@@ -1318,45 +1601,46 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>86</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="8" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
String Functions CONCAT SUBSTRING REVERSE CHAR_LENGTH
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E28EDC-0D83-4630-B6EA-5E02D3B59E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85518C79-1297-448E-8C71-64925FF0AF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="144">
   <si>
     <t>Name</t>
   </si>
@@ -678,6 +678,281 @@
   </si>
   <si>
     <t>SELECT concat(author_fname, " " ,author_lname)  as "Full name" FROM books</t>
+  </si>
+  <si>
+    <t>substring()</t>
+  </si>
+  <si>
+    <t>SELECT substring("Hello World", 7) as word</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>SELECT substring("Hello World", 1,7) as word</t>
+  </si>
+  <si>
+    <t>Hello W</t>
+  </si>
+  <si>
+    <t>SELECT substring("Hello World", -3) as word</t>
+  </si>
+  <si>
+    <t>rld</t>
+  </si>
+  <si>
+    <r>
+      <t>Here</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Title </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is column name</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT substring(title, 1,15) as "short title" FROM books</t>
+  </si>
+  <si>
+    <t>Combining Concat() and Substring()</t>
+  </si>
+  <si>
+    <t>SELECT concat(substring(title, 1,15), "...") as 'short title' FROM books</t>
+  </si>
+  <si>
+    <t>replace()</t>
+  </si>
+  <si>
+    <t>It is case sensitive and can replace multiple substrings that are matched</t>
+  </si>
+  <si>
+    <r>
+      <t>SELECT REPLACE(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Hello World'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Hell'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'%$#@'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SELECT REPLACE(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Hello World'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'o'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'0'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SELECT REPLACE(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'HellO World'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'o'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'*'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>"HellO W*rld"</t>
+  </si>
+  <si>
+    <t>"Hell0 W0rld"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple </t>
+  </si>
+  <si>
+    <t>Case sensitive</t>
+  </si>
+  <si>
+    <t>SELECT SUBSTRING(REPLACE(title, 'e', '3'), 1, 10) FROM books;</t>
+  </si>
+  <si>
+    <t>Combining with other string methods</t>
+  </si>
+  <si>
+    <t>reverse()</t>
+  </si>
+  <si>
+    <t>SELECT REVERSE("hello world")</t>
+  </si>
+  <si>
+    <t>CHAR_LENGTH()</t>
+  </si>
+  <si>
+    <t>SELECT CHAR_LENGTH("Hello World")</t>
+  </si>
+  <si>
+    <t>SELECT title, CHAR_LENGTH(title) as length FROM books</t>
   </si>
 </sst>
 </file>
@@ -1566,29 +1841,146 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05725D4A-CABB-4097-BFF4-F1E5D461FA05}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
String Functions CONCAT SUBSTRING REVERSE CHAR_LENGTH UPPER LOWER
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85518C79-1297-448E-8C71-64925FF0AF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A186FA7-A7AE-490C-A3D3-008CCC81ED41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -953,6 +953,12 @@
   </si>
   <si>
     <t>SELECT title, CHAR_LENGTH(title) as length FROM books</t>
+  </si>
+  <si>
+    <t>UPPER()</t>
+  </si>
+  <si>
+    <t>LOWER()</t>
   </si>
 </sst>
 </file>
@@ -1841,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05725D4A-CABB-4097-BFF4-F1E5D461FA05}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,6 +1987,16 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SELECT query with DISTINCT LIMIT LIKE ORDER BY keywords
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A186FA7-A7AE-490C-A3D3-008CCC81ED41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC76ED0-7094-4ADD-A524-F138AA8FCF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="158">
   <si>
     <t>Name</t>
   </si>
@@ -959,6 +959,65 @@
   </si>
   <si>
     <t>LOWER()</t>
+  </si>
+  <si>
+    <r>
+      <t>SELECT DISTINCT CONCAT(author_fname,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, author_lname) FROM books;</t>
+    </r>
+  </si>
+  <si>
+    <t>DISTINCT with Concat()</t>
+  </si>
+  <si>
+    <t>SELECT title, author_fname, author_lname 
+FROM books ORDER BY 1;</t>
+  </si>
+  <si>
+    <t>SELECT author_fname, author_lname FROM books 
+ORDER BY author_lname, author_fname;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM tbl LIMIT 95,18446744073709551615;</t>
+  </si>
+  <si>
+    <t>returning output from an offset to all the remaining rows. Use some big number more than no of rows</t>
+  </si>
+  <si>
+    <t>SELECT * FROM books WHERE author_fname LIKE "%Da%"</t>
+  </si>
+  <si>
+    <t>Da anywhere</t>
+  </si>
+  <si>
+    <t>Da at starting</t>
+  </si>
+  <si>
+    <t>SELECT title FROM books WHERE title LIKE '%\%%'
+SELECT title FROM books WHERE title LIKE '%\_%'</t>
+  </si>
+  <si>
+    <t>SELECT * FROM books WHERE author_fname LIKE "Da%"</t>
+  </si>
+  <si>
+    <t>When we have % and _ as values</t>
   </si>
 </sst>
 </file>
@@ -1388,11 +1447,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,313 +1588,378 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="6" t="s">
-        <v>26</v>
+      <c r="B15" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="12" t="s">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="8" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8" t="s">
+    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="D28" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="B32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="B34" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="B35" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="B37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D46" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>97</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D47" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>111</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C51" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D51" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1849,7 +1973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05725D4A-CABB-4097-BFF4-F1E5D461FA05}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Aggregate Function GROUP BY, SUM, MIN and MAX
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230BD24E-3FC3-45C8-AE8F-1ABBB6E83171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDB2261-00DE-4DF9-A53F-2B0D02D22301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="183">
   <si>
     <t>Name</t>
   </si>
@@ -1060,6 +1060,123 @@
       </rPr>
       <t>;</t>
     </r>
+  </si>
+  <si>
+    <t>Count()</t>
+  </si>
+  <si>
+    <t>GROUP BY</t>
+  </si>
+  <si>
+    <t>SELECT Concat(author_fname, " ", author_lname) AS "Full name", COUNT(*) FROM books GROUP BY author_fname, author_lname</t>
+  </si>
+  <si>
+    <t>SELECT author_fname, author_lname, COUNT(*) FROM books GROUP BY author_fname, author_lname</t>
+  </si>
+  <si>
+    <r>
+      <t>SELECT CONCAT(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'In '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, released_year, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, COUNT(*), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2D907F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' book(s) released'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) AS year FROM books GROUP BY released_year;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MIN() and MAX() </t>
+  </si>
+  <si>
+    <t>SELECT MIN(released_year) FROM books</t>
+  </si>
+  <si>
+    <t>SELECT MAX(released_year) FROM books</t>
+  </si>
+  <si>
+    <t>SELECT title FROM books WHERE pages = (SELECT MAX(pages) FROM books) - CORRECT
+SELECT MAX(pages) FROM books if we want title of MAX pages and if we exeute SELECT MAX(pages), title FROM books it gives a wrong result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficient Query is below because it executes only one query
+SELECT title, pages FROM books ORDER BY pages ASC LIMIT 1;
+</t>
+  </si>
+  <si>
+    <t>MIN max with GROUP</t>
+  </si>
+  <si>
+    <t>SELECT author_fname, author_lname, MIN(released_year) FROM books GROUP BY author_fname, author_lname</t>
+  </si>
+  <si>
+    <t># Find the year each author published their first book</t>
+  </si>
+  <si>
+    <t># Find the title name of max pages each author published 
+#SELECT author_fname, author_lname, MAX(pages) FROM books GROUP BY author_fname, author_lname
+-- Not working
+#SELECT title FROM books
+#WHERE pages= (SELECT MAX(pages) FROM books GROUP BY author_fname, author_lname)</t>
+  </si>
+  <si>
+    <t>SOLVE this Question</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>SELECT SUM(pages) FROM books;</t>
+  </si>
+  <si>
+    <t>SELECT author_fname, author_lname, Sum(pages) FROM books GROUP BY author_lname, author_fname;</t>
   </si>
 </sst>
 </file>
@@ -1492,8 +1609,8 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="C1:D2"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,16 +2293,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63968E43-EBAC-446A-A670-BEF2F9484100}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2200,6 +2317,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
       <c r="B2" t="s">
         <v>160</v>
       </c>
@@ -2222,6 +2342,83 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="20" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data types CHAR, VARCHAR, DECIMAL, FLOAT, DOUBLE, DATE, TIME, DATETIME topics
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDB2261-00DE-4DF9-A53F-2B0D02D22301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339B55E8-FF48-44EA-BE4A-4FDC5C6768D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="1" r:id="rId1"/>
     <sheet name="String Functions" sheetId="3" r:id="rId2"/>
     <sheet name="Aggregate Functions" sheetId="4" r:id="rId3"/>
     <sheet name="Notes" sheetId="2" r:id="rId4"/>
+    <sheet name="Table notes" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="209">
   <si>
     <t>Name</t>
   </si>
@@ -1177,6 +1178,85 @@
   </si>
   <si>
     <t>SELECT author_fname, author_lname, Sum(pages) FROM books GROUP BY author_lname, author_fname;</t>
+  </si>
+  <si>
+    <t>Data types</t>
+  </si>
+  <si>
+    <t>CHAR</t>
+  </si>
+  <si>
+    <t>Fixed length of character. Even if we use full length of charcters or not. Memory will be allocated.
+CHAR best suits for fixed length Characters filed values live - SEX:M/F, Yes or No, etc</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>Fixed Length of character can be assigend and uses memeory as per values of fields</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>Decimal(5,2) - 5 represents all digits inculing decimal values. 2 represent decimal values. IT is a FIXED Point type. If precision DOESN'T matter Use decimal else use FLOAT or DOUBLE</t>
+  </si>
+  <si>
+    <t>Memory 4 bytes. Precision issue ~ 7</t>
+  </si>
+  <si>
+    <t>Memory 8 bytes. Precision issue ~ 15</t>
+  </si>
+  <si>
+    <t>Formating dates</t>
+  </si>
+  <si>
+    <t>Date Math</t>
+  </si>
+  <si>
+    <t>Working with Timestamps</t>
+  </si>
+  <si>
+    <t>DATE - 'YYYY-MM-DD'</t>
+  </si>
+  <si>
+    <t>TIME - 'HH:MM:SS'</t>
+  </si>
+  <si>
+    <t>Datetime - 'YYYY-MM-DD HH:MM:SS'</t>
+  </si>
+  <si>
+    <t>CURDATE()</t>
+  </si>
+  <si>
+    <t>CURTIME()</t>
+  </si>
+  <si>
+    <t>NOW()</t>
+  </si>
+  <si>
+    <t>Gives Current date</t>
+  </si>
+  <si>
+    <t>Gives Current time</t>
+  </si>
+  <si>
+    <t>Gives Current datetime</t>
+  </si>
+  <si>
+    <t>INSERT INTO family (name, birthdate, birthtime, birthdt) VALUES ("Surya Kumari", "1950-12-15", "05:05:30", "1950-12-15 05:05:30")</t>
+  </si>
+  <si>
+    <t>CREATE TABLE family (id INT AUTO_INCREMENT PRIMARY KEY, name VARCHAR(50), birthdate DATE, birthtime TIME, birthdt DATETIME)</t>
+  </si>
+  <si>
+    <t>INSERT INTO family (name, birthdate, birthtime, birthdt) VALUES ("Lovely", CURDATE(), CURTIME(), NOW())</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1271,11 +1351,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1326,6 +1430,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2295,7 +2403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63968E43-EBAC-446A-A670-BEF2F9484100}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
@@ -2429,10 +2537,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A372CFD-6369-4C1F-9C7A-9162FAE256E2}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C1" sqref="C1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,64 +2549,31 @@
     <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="18"/>
-      <c r="C2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="18"/>
-      <c r="C3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="18"/>
-      <c r="C4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="18"/>
-      <c r="C5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>65</v>
       </c>
@@ -2506,7 +2581,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -2514,13 +2589,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>86</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>101</v>
       </c>
@@ -2528,7 +2603,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>100</v>
       </c>
@@ -2536,7 +2611,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>99</v>
       </c>
@@ -2548,4 +2623,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EAE72C-AF07-4B08-A3A7-DD49A8E103B6}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="122.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="E1" s="22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="E2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DATA Types timestamp. Logical Operators
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339B55E8-FF48-44EA-BE4A-4FDC5C6768D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDCB62D-05A6-4FB3-9085-3CBE137AE1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="String Functions" sheetId="3" r:id="rId2"/>
     <sheet name="Aggregate Functions" sheetId="4" r:id="rId3"/>
     <sheet name="Notes" sheetId="2" r:id="rId4"/>
-    <sheet name="Table notes" sheetId="5" r:id="rId5"/>
+    <sheet name="Logical Operators" sheetId="6" r:id="rId5"/>
+    <sheet name="Table notes" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -1258,12 +1259,653 @@
   <si>
     <t>INSERT INTO family (name, birthdate, birthtime, birthdt) VALUES ("Lovely", CURDATE(), CURTIME(), NOW())</t>
   </si>
+  <si>
+    <t>DATE: 2021-09-13 
+DAY() - Gives only date. Ex: 13 , 
+DAYNAME() - Gives weekname. Ex: Monday, 
+DAYOFWEEK() - Gives weeknumber. Ex: 2, 
+DAYOFYEAR() - Gives day count in year. Ex: 156
+MONTHNAME() - Gives Month name. Ex: September</t>
+  </si>
+  <si>
+    <t>Specifier</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>%a</t>
+  </si>
+  <si>
+    <t>%b</t>
+  </si>
+  <si>
+    <t>%c</t>
+  </si>
+  <si>
+    <t>%D</t>
+  </si>
+  <si>
+    <t>%d</t>
+  </si>
+  <si>
+    <t>%e</t>
+  </si>
+  <si>
+    <t>%f</t>
+  </si>
+  <si>
+    <t>%H</t>
+  </si>
+  <si>
+    <t>%h</t>
+  </si>
+  <si>
+    <t>%I</t>
+  </si>
+  <si>
+    <t>%i</t>
+  </si>
+  <si>
+    <t>%j</t>
+  </si>
+  <si>
+    <t>%k</t>
+  </si>
+  <si>
+    <t>%l</t>
+  </si>
+  <si>
+    <t>%M</t>
+  </si>
+  <si>
+    <t>%m</t>
+  </si>
+  <si>
+    <t>%p</t>
+  </si>
+  <si>
+    <t>%r</t>
+  </si>
+  <si>
+    <t>%S</t>
+  </si>
+  <si>
+    <t>%s</t>
+  </si>
+  <si>
+    <t>%T</t>
+  </si>
+  <si>
+    <t>%U</t>
+  </si>
+  <si>
+    <t>Week (00..53), where Sunday is the first day of the week; WEEK() mode 0</t>
+  </si>
+  <si>
+    <t>%u</t>
+  </si>
+  <si>
+    <t>Week (00..53), where Monday is the first day of the week; WEEK() mode 1</t>
+  </si>
+  <si>
+    <t>%V</t>
+  </si>
+  <si>
+    <t>Week (01..53), where Sunday is the first day of the week; WEEK() mode 2; used with %X</t>
+  </si>
+  <si>
+    <t>%v</t>
+  </si>
+  <si>
+    <t>Week (01..53), where Monday is the first day of the week; WEEK() mode 3; used with %x</t>
+  </si>
+  <si>
+    <t>%W</t>
+  </si>
+  <si>
+    <t>%w</t>
+  </si>
+  <si>
+    <t>%X</t>
+  </si>
+  <si>
+    <t>%x</t>
+  </si>
+  <si>
+    <t>%Y</t>
+  </si>
+  <si>
+    <t>Year, numeric, four digits</t>
+  </si>
+  <si>
+    <t>%y</t>
+  </si>
+  <si>
+    <t>Year, numeric (two digits)</t>
+  </si>
+  <si>
+    <t>%%</t>
+  </si>
+  <si>
+    <t>Abbreviated weekday name (Sun..Sat)</t>
+  </si>
+  <si>
+    <t>Abbreviated month name (Jan..Dec)</t>
+  </si>
+  <si>
+    <t>Month, numeric (0..12)</t>
+  </si>
+  <si>
+    <t>Day of the month with English suffix (0th, 1st, 2nd, 3rd, …)</t>
+  </si>
+  <si>
+    <t>Day of the month, numeric (00..31)</t>
+  </si>
+  <si>
+    <t>Day of the month, numeric (0..31)</t>
+  </si>
+  <si>
+    <t>Microseconds (000000..999999)</t>
+  </si>
+  <si>
+    <t>Hour (00..23)</t>
+  </si>
+  <si>
+    <t>Hour (01..12)</t>
+  </si>
+  <si>
+    <t>Minutes, numeric (00..59)</t>
+  </si>
+  <si>
+    <t>Day of year (001..366)</t>
+  </si>
+  <si>
+    <t>Hour (0..23)</t>
+  </si>
+  <si>
+    <t>Hour (1..12)</t>
+  </si>
+  <si>
+    <t>Month name (January..December)</t>
+  </si>
+  <si>
+    <t>Month, numeric (00..12)</t>
+  </si>
+  <si>
+    <t>AM or PM</t>
+  </si>
+  <si>
+    <t>Seconds (00..59)</t>
+  </si>
+  <si>
+    <t>Weekday name (Sunday..Saturday)</t>
+  </si>
+  <si>
+    <t>Day of the week (0=Sunday..6=Saturday)</t>
+  </si>
+  <si>
+    <t>Year for the week where Sunday is the first day of the week, numeric, four digits; used with %V</t>
+  </si>
+  <si>
+    <t>Year for the week, where Monday is the first day of the week, numeric, four digits; used with %v</t>
+  </si>
+  <si>
+    <t>A literal % character</t>
+  </si>
+  <si>
+    <r>
+      <t>Time, 12-hour (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hh:mm:ss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> followed by AM or PM)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Time, 24-hour (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hh:mm:ss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, for any “</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>” not listed above</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DATE_FORMAT() </t>
+  </si>
+  <si>
+    <t>DATE_FORMAT() function is best to use while working with date instead of using each function above for each value.
+SELECT DATE_FORMAT(birthdate, "%W") FROM family
+SELECT DATE_FORMAT(birthdt, '%m/%d/%Y') FROM family
+SELECT DATE_FORMAT(birthdt, '%m/%d/%Y at %h:%i') FROM family</t>
+  </si>
+  <si>
+    <t>DATEDIFF() - SELECT DATEDIFF(now(), birthdate) FROM family
+DATE_ADD() - SELECT birthdt, DATE_ADD(birthdt, INTERVAL 1 MONTH) FROM people;</t>
+  </si>
+  <si>
+    <t>Timestamp in MYSQL works only between 1970 to 2038 years only</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE TABLE comments (
+    content VARCHAR(100),
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> created_at TIMESTAMP DEFAULT NOW()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+);
+INSERT INTO comments (content) VALUES('lol what a funny article');</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE TABLE comments2 (
+    content VARCHAR(100),
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">changed_at TIMESTAMP DEFAULT NOW() ON UPDATE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CURRENT_TIMESTAMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+);
+INSERT INTO comments2 (content) VALUES('dasdasdasd');
+INSERT INTO comments2 (content) VALUES('lololololo');
+INSERT INTO comments2 (content) VALUES('I LIKE CATS AND DOGS');
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UPDATE comments2 SET content='THIS IS NOT GIBBERISH' WHERE content='dasdasdasd';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SELECT * FROM comments2;
+SELECT * FROM comments2 ORDER BY changed_at;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CREATE TABLE comments2 (
+    content VARCHAR(100),
+    changed_at TIMESTAMP DEFAULT NOW() ON UPDATE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOW()</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+);</t>
+    </r>
+  </si>
+  <si>
+    <t>Logical Operators</t>
+  </si>
+  <si>
+    <t>Not Equal</t>
+  </si>
+  <si>
+    <t>!=</t>
+  </si>
+  <si>
+    <t>Not Like</t>
+  </si>
+  <si>
+    <t>NOT LIKE</t>
+  </si>
+  <si>
+    <t>SELECT title, released_year FROM books 
+WHERE released_year &gt; 2000 ORDER BY released_year;
+SELECT * FROM books WHERE stock_quantity&gt;=200;</t>
+  </si>
+  <si>
+    <t>&gt; 
+&gt;=</t>
+  </si>
+  <si>
+    <t>Greater Than
+Greater Than equal to</t>
+  </si>
+  <si>
+    <t>Less Than
+Less Than equal to</t>
+  </si>
+  <si>
+    <t>&lt;
+&lt;=</t>
+  </si>
+  <si>
+    <t>SELECT title, released_year FROM books WHERE released_year &lt; 2000;
+SELECT title, released_year FROM books
+WHERE released_year &lt;= 2000;</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>In And Not In</t>
+  </si>
+  <si>
+    <t>Case Statement</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>AND
+&amp;&amp;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT title FROM books WHERE title LIKE 'W%'; 
+SELECT title FROM books WHERE title </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOT LIKE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'W%';</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT title FROM books WHERE released_year </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2017;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Both AND and &amp;&amp; gives same results:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SELECT * FROM books WHERE author_lname = "eggers" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> released_year&gt;2010;
+SELECT * FROM books WHERE author_lname = "eggers" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> released_year&gt;2010;
+More than once we can use in same query:
+SELECT * FROM books WHERE author_lname='Eggers' 
+    AND released_year &gt; 2010 
+    AND title LIKE '%novel%';</t>
+    </r>
+  </si>
+  <si>
+    <t>OR
+||</t>
+  </si>
+  <si>
+    <t>SELECT title, author_lname, released_year FROM books
+WHERE author_lname='Eggers' || released_year &gt; 2010;</t>
+  </si>
+  <si>
+    <t>BETWEEN value AND value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1291,8 +1933,53 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1302,6 +1989,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1376,10 +2069,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1434,8 +2128,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1717,8 +2428,8 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,20 +3337,147 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EAE72C-AF07-4B08-A3A7-DD49A8E103B6}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1B49F6-D5E2-46ED-AEAA-B889D4BBD959}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EAE72C-AF07-4B08-A3A7-DD49A8E103B6}">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="122.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>107</v>
       </c>
@@ -2648,8 +3486,14 @@
       <c r="E1" s="22" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H1" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -2661,8 +3505,14 @@
       <c r="F2" s="8" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>81</v>
       </c>
@@ -2678,8 +3528,14 @@
       <c r="F3" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>90</v>
       </c>
@@ -2693,8 +3549,14 @@
       <c r="F4" s="8" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
@@ -2706,82 +3568,325 @@
       <c r="F5" s="7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E6" s="10" t="s">
         <v>190</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" s="23" t="s">
         <v>197</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="23" t="s">
         <v>198</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="10" t="s">
         <v>199</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10" s="10" t="s">
+      <c r="H9" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="12" t="s">
         <v>200</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="10" t="s">
+      <c r="H10" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="12" t="s">
         <v>201</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" s="10" t="s">
+      <c r="H11" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="12" t="s">
         <v>202</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="E13" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="10" t="s">
+      <c r="F13" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E14" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F16" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="F17" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" ht="315" x14ac:dyDescent="0.25">
+      <c r="F18" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H19" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H23" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H24" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H25" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H26" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="29" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H29" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="6:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H30" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="I33" s="25" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>275</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I23" r:id="rId1" location="function_week" display="https://dev.mysql.com/doc/refman/8.0/en/date-and-time-functions.html - function_week" xr:uid="{8381645C-CDA3-4682-BF11-1460454BBC1E}"/>
+    <hyperlink ref="I24" r:id="rId2" location="function_week" display="https://dev.mysql.com/doc/refman/8.0/en/date-and-time-functions.html - function_week" xr:uid="{C898D3CF-BC70-47CF-AD6B-650FC7FDE1CB}"/>
+    <hyperlink ref="I25" r:id="rId3" location="function_week" display="https://dev.mysql.com/doc/refman/8.0/en/date-and-time-functions.html - function_week" xr:uid="{12B12BEB-0B91-4CBC-969B-BBE8F6469E88}"/>
+    <hyperlink ref="I26" r:id="rId4" location="function_week" display="https://dev.mysql.com/doc/refman/8.0/en/date-and-time-functions.html - function_week" xr:uid="{786DC2B4-6C13-40CC-BFE6-8310F92D5CAE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IFNULL, ON DELETE CASCADE, JOINS practice[C
</commit_message>
<xml_diff>
--- a/MYSQL.xlsx
+++ b/MYSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Mysql\SQL-quering-with-MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F66E866-8990-4FB0-9CB8-FD5BA5DF2897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F94662-2437-4C2B-B28C-69C01C87D071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="327">
   <si>
     <t>Name</t>
   </si>
@@ -440,9 +440,6 @@
   </si>
   <si>
     <t>To delete table</t>
-  </si>
-  <si>
-    <t>DROP DATABASE mydabase</t>
   </si>
   <si>
     <t>DROP TABLE mytable</t>
@@ -2130,6 +2127,81 @@
       <t xml:space="preserve">
 );</t>
     </r>
+  </si>
+  <si>
+    <t>DROP DATABASE mydatabase</t>
+  </si>
+  <si>
+    <t>12. IFNULL(fieldname, value we want to fill)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT 
+    first_name, 
+    last_name,
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IFNULL(SUM(amount), 0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> AS total_spent
+FROM customers
+LEFT JOIN orders
+    ON customers.id = orders.customer_id</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE TABLE orders(
+    id INT AUTO_INCREMENT PRIMARY KEY,
+    order_date DATE,
+    amount DECIMAL(8,2),
+    customer_id INT,
+    FOREIGN KEY(customer_id) 
+        REFERENCES customers(id)
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ON DELETE CASCADE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+);</t>
+    </r>
+  </si>
+  <si>
+    <t>13. ON DELETE CASCADE - Helps in deleting rows in existing when forigen key values are deleted in main table. Refer to CODE: Right Joins Part 2</t>
   </si>
 </sst>
 </file>
@@ -2310,7 +2382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2383,6 +2455,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2668,8 +2746,8 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2723,7 +2801,7 @@
         <v>75</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2745,7 +2823,7 @@
         <v>71</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2757,7 +2835,7 @@
         <v>76</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>78</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2767,7 +2845,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2810,10 +2888,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2894,30 +2972,30 @@
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="6"/>
       <c r="C20" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -2961,7 +3039,7 @@
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2969,7 +3047,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2995,10 +3073,10 @@
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -3091,14 +3169,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3106,7 +3184,7 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3117,14 +3195,14 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3132,53 +3210,53 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3192,7 +3270,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,125 +3283,125 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>113</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
         <v>119</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
         <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
         <v>125</v>
-      </c>
-      <c r="B8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" t="s">
         <v>127</v>
-      </c>
-      <c r="B10" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
         <v>133</v>
-      </c>
-      <c r="D12" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
         <v>131</v>
       </c>
-      <c r="C13" t="s">
-        <v>132</v>
-      </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" t="s">
         <v>138</v>
-      </c>
-      <c r="B16" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" t="s">
         <v>140</v>
-      </c>
-      <c r="B17" t="s">
-        <v>141</v>
       </c>
       <c r="C17">
         <v>11</v>
@@ -3331,17 +3409,17 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -3355,7 +3433,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B26"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3366,118 +3444,118 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s">
         <v>169</v>
-      </c>
-      <c r="B13" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3488,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A372CFD-6369-4C1F-9C7A-9162FAE256E2}">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,48 +3612,64 @@
     </row>
     <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>322</v>
+    </row>
+    <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3588,8 +3682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1B49F6-D5E2-46ED-AEAA-B889D4BBD959}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3601,76 +3695,76 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>283</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>285</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>290</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3678,82 +3772,82 @@
         <v>27</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>304</v>
-      </c>
       <c r="C9" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>309</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>312</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3766,8 +3860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EAE72C-AF07-4B08-A3A7-DD49A8E103B6}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3783,18 +3877,18 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="E1" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H1" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="I1" s="23" t="s">
         <v>209</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3804,383 +3898,383 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>184</v>
-      </c>
       <c r="H2" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="E3" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="H3" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="E5" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E6" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="E13" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="E14" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>276</v>
-      </c>
       <c r="H14" s="24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E15" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="6:9" ht="90" x14ac:dyDescent="0.25">
       <c r="F17" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="6:9" ht="315" x14ac:dyDescent="0.25">
       <c r="F18" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="6:9" ht="30" x14ac:dyDescent="0.25">
       <c r="H19" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H20" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H21" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H22" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="6:9" ht="30" x14ac:dyDescent="0.25">
       <c r="H23" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="I23" s="25" t="s">
         <v>232</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="24" spans="6:9" ht="30" x14ac:dyDescent="0.25">
       <c r="H24" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="I24" s="25" t="s">
         <v>234</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="25" spans="6:9" ht="30" x14ac:dyDescent="0.25">
       <c r="H25" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="I25" s="25" t="s">
         <v>236</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="26" spans="6:9" ht="30" x14ac:dyDescent="0.25">
       <c r="H26" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="I26" s="25" t="s">
         <v>238</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="27" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H27" s="24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H28" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="6:9" ht="30" x14ac:dyDescent="0.25">
       <c r="H29" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="6:9" ht="45" x14ac:dyDescent="0.25">
       <c r="H30" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H31" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="I31" s="24" t="s">
         <v>244</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="32" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H32" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="I32" s="24" t="s">
         <v>246</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="I34" s="26" t="s">
         <v>273</v>
-      </c>
-      <c r="I34" s="26" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>